<commit_message>
Qa add note to balloters for vte
</commit_message>
<xml_diff>
--- a/source/capstat_spreadsheets/DEQM_Capability_Statement_Receiver_Server.xlsx
+++ b/source/capstat_spreadsheets/DEQM_Capability_Statement_Receiver_Server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\capstat_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74112FF-031F-4985-A165-D6EAC6790050}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6847694-F310-49D3-8F08-A6C00DC9E3B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
   <si>
     <t>Value</t>
   </si>
@@ -288,12 +288,6 @@
   </si>
   <si>
     <t>QI Core</t>
-  </si>
-  <si>
-    <t>collect-data</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/OperationDefinition/collect-data</t>
   </si>
   <si>
     <t xml:space="preserve">Da Vinci DEQM Receiver Server **SHALL**
@@ -329,18 +323,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -374,27 +360,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,13 +374,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -725,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +714,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -756,7 +722,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +746,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -822,15 +788,15 @@
         <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B139EF60-0633-48C5-B394-C56F006BD6B3}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -1072,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1089,10 +1055,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1068,7 @@
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1116,26 +1082,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8E795EC9-A372-B646-AB2C-DC254C6245BD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1160,7 +1109,7 @@
         <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>